<commit_message>
feat: try to evaluate with ragas
</commit_message>
<xml_diff>
--- a/test/adaptive/results/score_ragas_adaptive_20241226212954_vdb1000200_optimization.xlsx
+++ b/test/adaptive/results/score_ragas_adaptive_20241226212954_vdb1000200_optimization.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\adaptive\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7FD5F6-353A-4511-B843-8A8BA529FC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="189">
   <si>
     <t>question</t>
   </si>
@@ -935,8 +941,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -988,25 +994,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1044,7 +1061,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1078,6 +1095,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1112,9 +1130,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1287,14 +1306,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1337,22 +1358,22 @@
         <v>158</v>
       </c>
       <c r="E2">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F2">
-        <v>0.8181818181818182</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.8820855704736031</v>
+        <v>0.88208557047360314</v>
       </c>
       <c r="I2">
-        <v>0.9250668471388553</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>0.92506684713885534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1387,7 @@
         <v>159</v>
       </c>
       <c r="E3">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F3">
         <v>0.75</v>
@@ -1375,13 +1396,13 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.9277397468613131</v>
+        <v>0.92773974686131311</v>
       </c>
       <c r="I3">
-        <v>0.9194349366903283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0.91943493669032827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1395,7 +1416,7 @@
         <v>160</v>
       </c>
       <c r="E4">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1404,13 +1425,13 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.8949485996578921</v>
+        <v>0.89494859965789209</v>
       </c>
       <c r="I4">
-        <v>0.973737149889473</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0.97373714988947302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1424,7 +1445,7 @@
         <v>112</v>
       </c>
       <c r="E5">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1433,13 +1454,13 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.8731718592731655</v>
+        <v>0.87317185927316554</v>
       </c>
       <c r="I5">
-        <v>0.9682929647932914</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0.96829296479329141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1453,7 +1474,7 @@
         <v>161</v>
       </c>
       <c r="E6">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1462,13 +1483,13 @@
         <v>0.8</v>
       </c>
       <c r="H6">
-        <v>0.8801839393933357</v>
+        <v>0.88018393939333572</v>
       </c>
       <c r="I6">
-        <v>0.9200459848233339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0.92004598482333388</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1497,7 +1518,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1511,7 +1532,7 @@
         <v>163</v>
       </c>
       <c r="E8">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1520,13 +1541,13 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0.8720651365928527</v>
+        <v>0.87206513659285267</v>
       </c>
       <c r="I8">
-        <v>0.9680162841232132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>0.96801628412321317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1540,7 +1561,7 @@
         <v>116</v>
       </c>
       <c r="E9">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1549,13 +1570,13 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.8545680179921812</v>
+        <v>0.85456801799218118</v>
       </c>
       <c r="I9">
-        <v>0.9636420044730453</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>0.96364200447304527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1569,7 +1590,7 @@
         <v>117</v>
       </c>
       <c r="E10">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1578,13 +1599,13 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0.910300409089277</v>
+        <v>0.91030040908927701</v>
       </c>
       <c r="I10">
-        <v>0.9775751022473192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>0.97757510224731925</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1598,7 +1619,7 @@
         <v>164</v>
       </c>
       <c r="E11">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F11">
         <v>0.8571428571428571</v>
@@ -1607,13 +1628,13 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0.8630329654276258</v>
+        <v>0.86303296542762575</v>
       </c>
       <c r="I11">
-        <v>0.9300439556176208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>0.93004395561762077</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1627,7 +1648,7 @@
         <v>119</v>
       </c>
       <c r="E12">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1636,13 +1657,13 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0.896001745909297</v>
+        <v>0.89600174590929704</v>
       </c>
       <c r="I12">
-        <v>0.9740004364523243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>0.97400043645232426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1671,7 +1692,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1685,7 +1706,7 @@
         <v>166</v>
       </c>
       <c r="E14">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1694,13 +1715,13 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.736457886939743</v>
+        <v>0.73645788693974301</v>
       </c>
       <c r="I14">
-        <v>0.9341144717099358</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>0.93411447170993578</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1714,7 +1735,7 @@
         <v>167</v>
       </c>
       <c r="E15">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1723,13 +1744,13 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0.8835136060947454</v>
+        <v>0.88351360609474539</v>
       </c>
       <c r="I15">
-        <v>0.9708784014986863</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>0.97087840149868632</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1743,7 +1764,7 @@
         <v>123</v>
       </c>
       <c r="E16">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1752,13 +1773,13 @@
         <v>0.5</v>
       </c>
       <c r="H16">
-        <v>0.8844306330813089</v>
+        <v>0.88443063308130887</v>
       </c>
       <c r="I16">
-        <v>0.8461076582453272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>0.84610765824532719</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1772,7 +1793,7 @@
         <v>168</v>
       </c>
       <c r="E17">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1781,13 +1802,13 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0.9330309089446568</v>
+        <v>0.93303090894465679</v>
       </c>
       <c r="I17">
-        <v>0.9832577272111642</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>0.98325772721116422</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1801,7 +1822,7 @@
         <v>125</v>
       </c>
       <c r="E18">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1810,13 +1831,13 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0.9466255387648529</v>
+        <v>0.94662553876485289</v>
       </c>
       <c r="I18">
-        <v>0.9866563846662132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>0.98665638466621319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1830,7 +1851,7 @@
         <v>126</v>
       </c>
       <c r="E19">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1839,13 +1860,13 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0.8910520927733142</v>
+        <v>0.89105209277331421</v>
       </c>
       <c r="I19">
-        <v>0.9727630231683285</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>0.97276302316832852</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1859,7 +1880,7 @@
         <v>169</v>
       </c>
       <c r="E20">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1868,13 +1889,13 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>0.8774408239401268</v>
+        <v>0.87744082394012679</v>
       </c>
       <c r="I20">
         <v>0.9693602059600317</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1888,7 +1909,7 @@
         <v>128</v>
       </c>
       <c r="E21">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1897,13 +1918,13 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>0.9345972679555867</v>
+        <v>0.93459726795558673</v>
       </c>
       <c r="I21">
-        <v>0.9836493169638967</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>0.98364931696389668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1917,7 +1938,7 @@
         <v>129</v>
       </c>
       <c r="E22">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1926,13 +1947,13 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>0.9203488747379381</v>
+        <v>0.92034887473793814</v>
       </c>
       <c r="I22">
-        <v>0.9800872186594846</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>0.98008721865948456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1946,7 +1967,7 @@
         <v>130</v>
       </c>
       <c r="E23">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1955,13 +1976,13 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>0.8864117557213446</v>
+        <v>0.88641175572134456</v>
       </c>
       <c r="I23">
-        <v>0.9716029389053361</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>0.97160293890533611</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1975,7 +1996,7 @@
         <v>131</v>
       </c>
       <c r="E24">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1984,13 +2005,13 @@
         <v>1</v>
       </c>
       <c r="H24">
-        <v>0.9455265265255962</v>
+        <v>0.94552652652559621</v>
       </c>
       <c r="I24">
-        <v>0.986381631606399</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>0.98638163160639902</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2004,7 +2025,7 @@
         <v>132</v>
       </c>
       <c r="E25">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2013,13 +2034,13 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <v>0.8791203348475</v>
+        <v>0.87912033484749996</v>
       </c>
       <c r="I25">
-        <v>0.969780083686875</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>0.96978008368687496</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2033,7 +2054,7 @@
         <v>170</v>
       </c>
       <c r="E26">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2042,13 +2063,13 @@
         <v>1</v>
       </c>
       <c r="H26">
-        <v>0.8692566917842486</v>
+        <v>0.86925669178424858</v>
       </c>
       <c r="I26">
-        <v>0.9673141729210621</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>0.96731417292106214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2062,7 +2083,7 @@
         <v>171</v>
       </c>
       <c r="E27">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2071,13 +2092,13 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <v>0.8866547060123562</v>
+        <v>0.88665470601235619</v>
       </c>
       <c r="I27">
-        <v>0.971663676478089</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>0.97166367647808904</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2091,7 +2112,7 @@
         <v>172</v>
       </c>
       <c r="E28">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2100,13 +2121,13 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <v>0.9446954709525647</v>
+        <v>0.94469547095256468</v>
       </c>
       <c r="I28">
-        <v>0.9861738677131412</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>0.98617386771314119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2120,7 +2141,7 @@
         <v>173</v>
       </c>
       <c r="E29">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2129,13 +2150,13 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>0.9304482439057717</v>
+        <v>0.93044824390577174</v>
       </c>
       <c r="I29">
-        <v>0.9826120609514429</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>0.98261206095144293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2149,7 +2170,7 @@
         <v>174</v>
       </c>
       <c r="E30">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F30">
         <v>0.5</v>
@@ -2158,13 +2179,13 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0.9400470933131028</v>
+        <v>0.94004709331310277</v>
       </c>
       <c r="I30">
-        <v>0.8600117733032757</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>0.86001177330327572</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2178,7 +2199,7 @@
         <v>175</v>
       </c>
       <c r="E31">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2190,10 +2211,10 @@
         <v>0.8525427503541968</v>
       </c>
       <c r="I31">
-        <v>0.9631356875635492</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>0.96313568756354917</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2207,7 +2228,7 @@
         <v>139</v>
       </c>
       <c r="E32">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2222,7 +2243,7 @@
         <v>0.9744284845911656</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2236,7 +2257,7 @@
         <v>176</v>
       </c>
       <c r="E33">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2245,27 +2266,27 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>0.9049090132202818</v>
+        <v>0.90490901322028183</v>
       </c>
       <c r="I33">
-        <v>0.9762272532800704</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>0.97622725328007043</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
       <c r="B34" t="s">
         <v>92</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E34">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2280,7 +2301,7 @@
         <v>0.749999999975</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2294,7 +2315,7 @@
         <v>177</v>
       </c>
       <c r="E35">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2303,13 +2324,13 @@
         <v>1</v>
       </c>
       <c r="H35">
-        <v>0.8909406807947572</v>
+        <v>0.89094068079475719</v>
       </c>
       <c r="I35">
-        <v>0.9727351701736893</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>0.97273517017368927</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -2323,7 +2344,7 @@
         <v>178</v>
       </c>
       <c r="E36">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2332,13 +2353,13 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>0.8872133843934673</v>
+        <v>0.88721338439346731</v>
       </c>
       <c r="I36">
-        <v>0.9718033460733668</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>0.97180334607336682</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -2352,7 +2373,7 @@
         <v>179</v>
       </c>
       <c r="E37">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2361,13 +2382,13 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <v>0.8725494772130221</v>
+        <v>0.87254947721302212</v>
       </c>
       <c r="I37">
-        <v>0.9681373692782556</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>0.96813736927825556</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -2381,7 +2402,7 @@
         <v>180</v>
       </c>
       <c r="E38">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2390,13 +2411,13 @@
         <v>1</v>
       </c>
       <c r="H38">
-        <v>0.8664484252049046</v>
+        <v>0.86644842520490462</v>
       </c>
       <c r="I38">
-        <v>0.9666121062762262</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>0.96661210627622618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -2410,7 +2431,7 @@
         <v>181</v>
       </c>
       <c r="E39">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F39">
         <v>0.8</v>
@@ -2419,13 +2440,13 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>0.949473316099697</v>
+        <v>0.94947331609969698</v>
       </c>
       <c r="I39">
-        <v>0.9373683289999242</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>0.93736832899992417</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -2439,7 +2460,7 @@
         <v>182</v>
       </c>
       <c r="E40">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2448,13 +2469,13 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0.887660499801212</v>
+        <v>0.88766049980121198</v>
       </c>
       <c r="I40">
-        <v>0.971915124925303</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>0.97191512492530296</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2468,7 +2489,7 @@
         <v>183</v>
       </c>
       <c r="E41">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2477,13 +2498,13 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>0.9571896233942686</v>
+        <v>0.95718962339426861</v>
       </c>
       <c r="I41">
-        <v>0.9892974058235672</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>0.98929740582356718</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -2497,7 +2518,7 @@
         <v>149</v>
       </c>
       <c r="E42">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -2509,10 +2530,10 @@
         <v>0.9695762024562814</v>
       </c>
       <c r="I42">
-        <v>0.9923940505890704</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>0.99239405058907038</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -2526,7 +2547,7 @@
         <v>150</v>
       </c>
       <c r="E43">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -2535,13 +2556,13 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0.9544831895884521</v>
+        <v>0.95448318958845213</v>
       </c>
       <c r="I43">
-        <v>0.9886207973721131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>0.98862079737211306</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -2555,7 +2576,7 @@
         <v>184</v>
       </c>
       <c r="E44">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2564,13 +2585,13 @@
         <v>1</v>
       </c>
       <c r="H44">
-        <v>0.9210039547348612</v>
+        <v>0.92100395473486119</v>
       </c>
       <c r="I44">
-        <v>0.9802509886587153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>0.98025098865871529</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -2584,7 +2605,7 @@
         <v>185</v>
       </c>
       <c r="E45">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2593,13 +2614,13 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>0.9176419950482601</v>
+        <v>0.91764199504826005</v>
       </c>
       <c r="I45">
-        <v>0.979410498737065</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>0.97941049873706498</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -2613,7 +2634,7 @@
         <v>153</v>
       </c>
       <c r="E46">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2622,13 +2643,13 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>0.9526155075560143</v>
+        <v>0.95261550755601432</v>
       </c>
       <c r="I46">
-        <v>0.9881538768640036</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>0.98815387686400358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -2642,7 +2663,7 @@
         <v>154</v>
       </c>
       <c r="E47">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2657,7 +2678,7 @@
         <v>0.9427902518880259</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -2671,7 +2692,7 @@
         <v>186</v>
       </c>
       <c r="E48">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -2680,13 +2701,13 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <v>0.8629161248457269</v>
+        <v>0.86291612484572688</v>
       </c>
       <c r="I48">
-        <v>0.9657290311864317</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>0.96572903118643172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2700,7 +2721,7 @@
         <v>187</v>
       </c>
       <c r="E49">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -2709,13 +2730,13 @@
         <v>0.8</v>
       </c>
       <c r="H49">
-        <v>0.8576752064847967</v>
+        <v>0.85767520648479667</v>
       </c>
       <c r="I49">
-        <v>0.9144188015961991</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>0.91441880159619915</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -2729,7 +2750,7 @@
         <v>188</v>
       </c>
       <c r="E50">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F50">
         <v>0.8</v>
@@ -2738,27 +2759,27 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>0.8453755853850723</v>
+        <v>0.84537558538507229</v>
       </c>
       <c r="I50">
         <v>0.911343896321268</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
       <c r="B51" t="s">
         <v>65</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D51" t="s">
         <v>114</v>
       </c>
       <c r="E51">
-        <v>0.9999999999</v>
+        <v>0.99999999989999999</v>
       </c>
       <c r="F51">
         <v>0.5</v>
@@ -2773,7 +2794,7 @@
         <v>0.624999999975</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>59</v>
       </c>
@@ -2781,19 +2802,19 @@
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53">
-        <v>0.959999999904</v>
+        <v>0.95999999990399998</v>
       </c>
       <c r="F53">
-        <v>0.9205064935064934</v>
+        <v>0.92050649350649338</v>
       </c>
       <c r="G53">
-        <v>0.982</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="H53">
-        <v>0.8232569265931469</v>
+        <v>0.82325692659314686</v>
       </c>
       <c r="I53">
-        <v>0.9214408550009101</v>
+        <v>0.92144085500091011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>